<commit_message>
adding interactions between tb and mdr-tb including relapse and reinfection
</commit_message>
<xml_diff>
--- a/resources/Method_TB.xlsx
+++ b/resources/Method_TB.xlsx
@@ -5,25 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Thanzi la Onse\TB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdm522\PycharmProjects\TLOmodel\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="731" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="731" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="DALY weights" sheetId="17" r:id="rId2"/>
     <sheet name="Structure" sheetId="2" r:id="rId3"/>
     <sheet name="parameters" sheetId="16" r:id="rId4"/>
-    <sheet name="Active_TB_summary" sheetId="4" r:id="rId5"/>
-    <sheet name="Active_TB_prob" sheetId="15" r:id="rId6"/>
-    <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId7"/>
-    <sheet name="Latent_TB_prob" sheetId="13" r:id="rId8"/>
-    <sheet name="References" sheetId="7" r:id="rId9"/>
+    <sheet name="details_rates" sheetId="18" r:id="rId5"/>
+    <sheet name="Active_TB_summary" sheetId="4" r:id="rId6"/>
+    <sheet name="Active_TB_prob" sheetId="15" r:id="rId7"/>
+    <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId8"/>
+    <sheet name="Latent_TB_prob" sheetId="13" r:id="rId9"/>
+    <sheet name="References" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7255" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7313" uniqueCount="153">
   <si>
     <t>Name:</t>
   </si>
@@ -349,9 +350,6 @@
     <t>tb_mortality_rate</t>
   </si>
   <si>
-    <t>tb_mortality_hiv</t>
-  </si>
-  <si>
     <t>williams_pnas2010</t>
   </si>
   <si>
@@ -466,6 +464,48 @@
   </si>
   <si>
     <t>Extensively drug-resistant HIV/AIDS - Tuberculosis with moderate anemia</t>
+  </si>
+  <si>
+    <t>rate_relapse_tx_complete</t>
+  </si>
+  <si>
+    <t>rate_relapse_tx_incomplete</t>
+  </si>
+  <si>
+    <t>rate_relapse_2yrs</t>
+  </si>
+  <si>
+    <t>juan_tableparams</t>
+  </si>
+  <si>
+    <t>monthly_probability</t>
+  </si>
+  <si>
+    <t>monthly_rate</t>
+  </si>
+  <si>
+    <t>tb_mortality_hiv_rate</t>
+  </si>
+  <si>
+    <t>monthly_prob_progr_active</t>
+  </si>
+  <si>
+    <t>ann_prob_self_cure</t>
+  </si>
+  <si>
+    <t>prop_self_cure</t>
+  </si>
+  <si>
+    <t>ann_prob_tb_mortality</t>
+  </si>
+  <si>
+    <t>ann_prob_relapse_tx_complete</t>
+  </si>
+  <si>
+    <t>ann_prob_relapse_tx_incomplete</t>
+  </si>
+  <si>
+    <t>ann_prob_relapse_2yrs</t>
   </si>
 </sst>
 </file>
@@ -748,16 +788,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>338019</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>318969</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>27927</xdr:rowOff>
+      <xdr:rowOff>199377</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -780,8 +820,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="802105" y="200526"/>
-          <a:ext cx="5952756" cy="6845822"/>
+          <a:off x="6534150" y="381000"/>
+          <a:ext cx="6072069" cy="7152627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -792,16 +832,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>484605</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66843</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>675105</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>200193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>20519</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>43279</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>211019</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>176629</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -824,12 +864,59 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6901447" y="66843"/>
-          <a:ext cx="5952756" cy="8799594"/>
+          <a:off x="12962355" y="409743"/>
+          <a:ext cx="6089114" cy="9196636"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>816610</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4445</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="https://documents.lucidchart.com/documents/839d8afd-2a2d-4593-a46b-5366392bee83/pages/0eqBfotfVGlV?a=746&amp;x=416&amp;y=113&amp;w=968&amp;h=532&amp;store=1&amp;accept=image%2F*&amp;auth=LCA%20fcf1c092c25b38547121baabf3be25cbe95a6f4a-ts%3D1554476654"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="628650"/>
+          <a:ext cx="5731510" cy="3147695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1278,11 +1365,59 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1290,7 +1425,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1298,240 +1433,240 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>106</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>116</v>
-      </c>
       <c r="D6" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="C8" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>123</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="C9" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="21" t="s">
         <v>130</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="D12" s="21" t="s">
         <v>130</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>123</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>126</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="D16" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="D17" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>123</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1546,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B47:C68"/>
   <sheetViews>
-    <sheetView zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1646,15 +1781,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.25" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,10 +1837,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="B4">
-        <v>1E-3</v>
+        <v>8.3329861207515066E-5</v>
       </c>
       <c r="F4" t="s">
         <v>71</v>
@@ -1727,7 +1863,7 @@
         <v>26.06</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,7 +1956,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="B14">
         <v>0.15</v>
@@ -1831,10 +1967,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="B15">
-        <v>0.33</v>
+        <v>2.7125317446546005E-2</v>
       </c>
       <c r="F15" t="s">
         <v>100</v>
@@ -1842,10 +1978,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="B16">
-        <v>0.15</v>
+        <v>1.2422199506118559E-2</v>
       </c>
       <c r="F16" t="s">
         <v>83</v>
@@ -1853,10 +1989,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="B17">
-        <v>0.84</v>
+        <v>6.7606180094051727E-2</v>
       </c>
       <c r="F17" t="s">
         <v>83</v>
@@ -1893,6 +2029,39 @@
       </c>
       <c r="F20" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21">
+        <v>2.6631142694990562E-3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22">
+        <v>1.1598875001476161E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23">
+        <v>1.2499218782546784E-4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1901,6 +2070,359 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>1E-3</v>
+      </c>
+      <c r="F4">
+        <f>B4/12</f>
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="G4">
+        <f>1-(EXP(-F4))</f>
+        <v>8.3329861207515066E-5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <v>3.44</v>
+      </c>
+      <c r="C5">
+        <v>6.76</v>
+      </c>
+      <c r="D5">
+        <v>13.28</v>
+      </c>
+      <c r="E5">
+        <v>26.06</v>
+      </c>
+      <c r="I5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6">
+        <v>0.35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7">
+        <v>0.63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>2.1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>2.9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11">
+        <v>2.6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13">
+        <v>0.68</v>
+      </c>
+      <c r="I13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14">
+        <v>0.15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15">
+        <v>0.33</v>
+      </c>
+      <c r="F15">
+        <f>B15/12</f>
+        <v>2.75E-2</v>
+      </c>
+      <c r="G15">
+        <f>1-EXP(-F15)</f>
+        <v>2.7125317446546005E-2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16">
+        <v>0.15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F23" si="0">B16/12</f>
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G23" si="1">1-EXP(-F16)</f>
+        <v>1.2422199506118559E-2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17">
+        <v>0.84</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>6.7606180094051727E-2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666666E-3</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>2.6631142694990562E-3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>1.1598875001476161E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1.25E-4</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1.2499218782546784E-4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -2340,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3435"/>
   <sheetViews>
@@ -70451,7 +70973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -70517,7 +71039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D163"/>
   <sheetViews>
@@ -72812,52 +73334,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="83.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updating tb infection and relapse
</commit_message>
<xml_diff>
--- a/resources/Method_TB.xlsx
+++ b/resources/Method_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="731" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="731" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7313" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7309" uniqueCount="152">
   <si>
     <t>Name:</t>
   </si>
@@ -254,9 +254,6 @@
     <t>transmission_rate</t>
   </si>
   <si>
-    <t>progression_to_active_rate</t>
-  </si>
-  <si>
     <t>horsburgh</t>
   </si>
   <si>
@@ -336,15 +333,6 @@
   </si>
   <si>
     <t>rel_infectiousness_hiv</t>
-  </si>
-  <si>
-    <t>prob_self_cure</t>
-  </si>
-  <si>
-    <t>rate_self_cure</t>
-  </si>
-  <si>
-    <t>tiemersma_plosOne2011</t>
   </si>
   <si>
     <t>tb_mortality_rate</t>
@@ -490,22 +478,31 @@
     <t>monthly_prob_progr_active</t>
   </si>
   <si>
-    <t>ann_prob_self_cure</t>
-  </si>
-  <si>
-    <t>prop_self_cure</t>
-  </si>
-  <si>
     <t>ann_prob_tb_mortality</t>
   </si>
   <si>
-    <t>ann_prob_relapse_tx_complete</t>
+    <t>ann_prob_tb_mortality_hiv</t>
   </si>
   <si>
-    <t>ann_prob_relapse_tx_incomplete</t>
+    <t>monthly_prob_relapse_tx_complete</t>
   </si>
   <si>
-    <t>ann_prob_relapse_2yrs</t>
+    <t>monthly_prob_relapse_tx_incomplete</t>
+  </si>
+  <si>
+    <t>monthly_prob_relapse_2yrs</t>
+  </si>
+  <si>
+    <t>annual_rate_self_cure</t>
+  </si>
+  <si>
+    <t>dye_1998_lancet</t>
+  </si>
+  <si>
+    <t>monthly_prob_self_cure</t>
+  </si>
+  <si>
+    <t>annual_progression_to_active_rate</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1422,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1433,240 +1430,240 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C18" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1781,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1798,16 +1795,16 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -1821,7 +1818,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1832,23 +1829,23 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>8.3329861207515066E-5</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>3.44</v>
@@ -1863,150 +1860,150 @@
         <v>26.06</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>0.35</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7">
         <v>0.63</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>2.1</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>2.9</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <v>2.6</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12">
         <v>1.5</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <v>0.68</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B14">
-        <v>0.15</v>
+        <v>1.6528546178382508E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B15">
-        <v>2.7125317446546005E-2</v>
+        <v>1.2422199506118559E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B16">
-        <v>1.2422199506118559E-2</v>
+        <v>6.7606180094051727E-2</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="B17">
-        <v>6.7606180094051727E-2</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18">
-        <v>1.8599999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2014,67 +2011,57 @@
         <v>79</v>
       </c>
       <c r="B19">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="B20">
-        <v>6.4000000000000001E-2</v>
+        <v>2.6631142694990562E-3</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B21">
-        <v>2.6631142694990562E-3</v>
+        <v>1.1598875001476161E-2</v>
       </c>
       <c r="F21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B22">
-        <v>1.1598875001476161E-2</v>
+        <v>1.2499218782546784E-4</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23">
-        <v>1.2499218782546784E-4</v>
-      </c>
-      <c r="F23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2089,22 +2076,22 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -2118,7 +2105,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2129,12 +2116,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
@@ -2148,12 +2135,12 @@
         <v>8.3329861207515066E-5</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>3.44</v>
@@ -2168,174 +2155,174 @@
         <v>26.06</v>
       </c>
       <c r="I5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>0.35</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7">
         <v>0.63</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>2.1</v>
       </c>
       <c r="I8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>2.9</v>
       </c>
       <c r="I10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <v>2.6</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12">
         <v>1.5</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <v>0.68</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="B14">
-        <v>0.15</v>
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <f>B14/12</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="G14">
+        <f>1-EXP(-F14)</f>
+        <v>1.6528546178382508E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15">
-        <v>0.33</v>
+        <v>0.15</v>
       </c>
       <c r="F15">
-        <f>B15/12</f>
-        <v>2.75E-2</v>
+        <f t="shared" ref="F15:F22" si="0">B15/12</f>
+        <v>1.2499999999999999E-2</v>
       </c>
       <c r="G15">
-        <f>1-EXP(-F15)</f>
-        <v>2.7125317446546005E-2</v>
+        <f t="shared" ref="G15:G22" si="1">1-EXP(-F15)</f>
+        <v>1.2422199506118559E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="B16">
-        <v>0.15</v>
+        <v>0.84</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F23" si="0">B16/12</f>
-        <v>1.2499999999999999E-2</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ref="G16:G23" si="1">1-EXP(-F16)</f>
-        <v>1.2422199506118559E-2</v>
-      </c>
-      <c r="I16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B17">
-        <v>0.84</v>
-      </c>
-      <c r="F17">
         <f t="shared" si="0"/>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G17">
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>6.7606180094051727E-2</v>
       </c>
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17">
+        <v>1.8599999999999998E-2</v>
+      </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18">
-        <v>1.8599999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2343,78 +2330,67 @@
         <v>79</v>
       </c>
       <c r="B19">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="B20">
-        <v>6.4000000000000001E-2</v>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666666E-3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>2.6631142694990562E-3</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21">
-        <v>3.2000000000000001E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>2.6666666666666666E-3</v>
+        <v>1.1666666666666667E-2</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>2.6631142694990562E-3</v>
+        <v>1.1598875001476161E-2</v>
       </c>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B22">
-        <v>0.14000000000000001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>1.1666666666666667E-2</v>
+        <v>1.25E-4</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>1.1598875001476161E-2</v>
+        <v>1.2499218782546784E-4</v>
       </c>
       <c r="I22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23">
-        <v>1.5E-3</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>1.25E-4</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="1"/>
-        <v>1.2499218782546784E-4</v>
-      </c>
-      <c r="I23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test runs done with tb testing algorithm
</commit_message>
<xml_diff>
--- a/resources/Method_TB.xlsx
+++ b/resources/Method_TB.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7309" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7310" uniqueCount="153">
   <si>
     <t>Name:</t>
   </si>
@@ -504,6 +504,9 @@
   <si>
     <t>annual_progression_to_active_rate</t>
   </si>
+  <si>
+    <t>probability</t>
+  </si>
 </sst>
 </file>
 
@@ -785,94 +788,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>318969</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>199377</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6534150" y="381000"/>
-          <a:ext cx="6072069" cy="7152627"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>675105</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>200193</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>211019</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>176629</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12962355" y="409743"/>
-          <a:ext cx="6089114" cy="9196636"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -880,7 +795,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>816610</xdr:colOff>
+      <xdr:colOff>807085</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>4445</xdr:rowOff>
     </xdr:to>
@@ -890,7 +805,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -914,6 +829,94 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>464833</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6229350" y="266700"/>
+          <a:ext cx="6522733" cy="6979934"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>29733</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>8401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13296900" y="266700"/>
+          <a:ext cx="7211583" cy="9171451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1679,7 +1682,7 @@
   <dimension ref="B47:C68"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1781,7 +1784,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1826,7 +1829,7 @@
         <v>69</v>
       </c>
       <c r="B3">
-        <v>4.9000000000000004</v>
+        <v>1E-3</v>
       </c>
       <c r="F3" t="s">
         <v>82</v>
@@ -2400,10 +2403,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2412,12 +2415,13 @@
     <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2436,8 +2440,11 @@
       <c r="F1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -2456,8 +2463,12 @@
       <c r="F2">
         <v>392</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>D2/E2</f>
+        <v>3.9556363950896661E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -2476,8 +2487,12 @@
       <c r="F3">
         <v>394</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G22" si="0">D3/E3</f>
+        <v>3.9330146052497369E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -2496,8 +2511,12 @@
       <c r="F4">
         <v>396</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>3.9954348826936161E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -2516,8 +2535,12 @@
       <c r="F5">
         <v>397</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>3.9718929401386287E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -2536,8 +2559,12 @@
       <c r="F6">
         <v>397</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>3.9444501507489961E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -2556,8 +2583,12 @@
       <c r="F7">
         <v>397</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3.9878184416817213E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -2576,8 +2607,12 @@
       <c r="F8">
         <v>392</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.9466055543484072E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -2596,8 +2631,12 @@
       <c r="F9">
         <v>383</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3.8292116686338942E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -2616,8 +2655,12 @@
       <c r="F10">
         <v>370</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3.713764345816206E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -2636,8 +2679,12 @@
       <c r="F11">
         <v>352</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>3.5339046207298031E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -2656,8 +2703,12 @@
       <c r="F12">
         <v>332</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3.2966101946351623E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -2676,8 +2727,12 @@
       <c r="F13">
         <v>312</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3.1354746449522891E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -2696,8 +2751,12 @@
       <c r="F14">
         <v>294</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2.9197433980408523E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -2716,8 +2775,12 @@
       <c r="F15">
         <v>261</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2.5939324782485191E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -2736,8 +2799,12 @@
       <c r="F16">
         <v>227</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>2.2848655544097378E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -2756,8 +2823,12 @@
       <c r="F17">
         <v>193</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1.9347194915648222E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -2771,7 +2842,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -2785,7 +2856,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -2799,7 +2870,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -2813,7 +2884,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2016</v>
       </c>
@@ -2831,6 +2902,10 @@
       </c>
       <c r="F22">
         <v>159</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1.6140109415570508E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2842,7 +2917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3435"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2219" sqref="F2219"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
tb - include referrals for treatment after testing
</commit_message>
<xml_diff>
--- a/resources/Method_TB.xlsx
+++ b/resources/Method_TB.xlsx
@@ -478,12 +478,6 @@
     <t>monthly_prob_progr_active</t>
   </si>
   <si>
-    <t>ann_prob_tb_mortality</t>
-  </si>
-  <si>
-    <t>ann_prob_tb_mortality_hiv</t>
-  </si>
-  <si>
     <t>monthly_prob_relapse_tx_complete</t>
   </si>
   <si>
@@ -506,6 +500,12 @@
   </si>
   <si>
     <t>probability</t>
+  </si>
+  <si>
+    <t>monthly_prob_tb_mortality</t>
+  </si>
+  <si>
+    <t>monthly_prob_tb_mortality_hiv</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1956,18 +1956,18 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14">
         <v>1.6528546178382508E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B15">
         <v>1.2422199506118559E-2</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B16">
         <v>6.7606180094051727E-2</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B20">
         <v>2.6631142694990562E-3</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B21">
         <v>1.1598875001476161E-2</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B22">
         <v>1.2499218782546784E-4</v>
@@ -2064,7 +2064,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G15" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14">
         <v>0.2</v>
@@ -2265,7 +2265,7 @@
         <v>1.6528546178382508E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
         <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tb - cure event after treatment
</commit_message>
<xml_diff>
--- a/resources/Method_TB.xlsx
+++ b/resources/Method_TB.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7310" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7312" uniqueCount="154">
   <si>
     <t>Name:</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>monthly_prob_tb_mortality_hiv</t>
+  </si>
+  <si>
+    <t>prob_treatment_sucess</t>
   </si>
 </sst>
 </file>
@@ -1781,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2050,6 +2053,17 @@
         <v>1.2499218782546784E-4</v>
       </c>
       <c r="F22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23">
+        <v>0.86</v>
+      </c>
+      <c r="F23" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>